<commit_message>
Update souce monitoring database info and note
</commit_message>
<xml_diff>
--- a/Others/Note_MonitoringMongoDB.xlsx
+++ b/Others/Note_MonitoringMongoDB.xlsx
@@ -10,13 +10,15 @@
     <sheet name="Index" sheetId="4" r:id="rId1"/>
     <sheet name="ServerStatus" sheetId="1" r:id="rId2"/>
     <sheet name="HostInfo" sheetId="3" r:id="rId3"/>
+    <sheet name="dbStats" sheetId="5" r:id="rId4"/>
+    <sheet name="collectionStats " sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="159">
   <si>
     <t>Note monitoring Mongodb (issue #386)</t>
   </si>
@@ -358,13 +360,184 @@
   </si>
   <si>
     <t>Monitoring host information</t>
+  </si>
+  <si>
+    <t>with command mongodb: db.hostInfo()</t>
+  </si>
+  <si>
+    <t>http://docs.mongodb.org/v2.4/reference/method/db.hostInfo/</t>
+  </si>
+  <si>
+    <t>version mongodb &gt; 2.2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MongoDB.HostInfo.System </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(about the underlying environment of the system running the mongod or mongos)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - currentTime (datetime): the current system time.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - hostname (string): The system name, which should correspond to the output of hostname -f on Linux systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cpuAddrSize (number): A number reflecting the architecture of the system. Either 32 or 64.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - memSizeMB (MB): The total amount of system memory (RAM) in megabytes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - numCores (number): The total number of available logical processor cores.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cpuArch (string): A string that represents the system architecture. Either x86 or x86_64.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - numaEnabled (boolean): false if NUMA is interleaved (i.e. disabled), otherwise true.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - type (string): A string representing the type of operating system, such as Linux or Windows.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - name (string): A display name for the operating system.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - version (string): The name of the distribution or operating system.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MongoDB.HostInfo.Extra </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(extra information about the operating system and the underlying hardware)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MongoDB.HostInfo.OS </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t>(A sub-document that contains information about the operating system running the mongod and mongos)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - versionString (string): A complete string of the operating system version and identification. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - libcVersion (string): The release of the system libc. libcVersion only appears on Linux systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - kernelVersion (string): The release of the Linux kernel in current use. kernelVersion only appears on Linux systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cpuFeatures (string): The processor feature flags. On Linux systems this the same information that /proc/cpuinfo includes in the flags fields.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cpuFrequencyMHz (string): The clock speed of the system’s processor in megahertz.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - pageSize (bytes): the default system page size in bytes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - numPages (page): numPages only appears on Linux systems.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - maxOpenFiles (number): The current system limits on open file handles. maxOpenFiles only appears on Linux systems.</t>
+  </si>
+  <si>
+    <t>Monitoring statistics for a given database</t>
+  </si>
+  <si>
+    <t>3. Monitoring statistics for a given database</t>
+  </si>
+  <si>
+    <t>http://docs.mongodb.org/v2.4/reference/command/dbStats/#dbcmd.dbStats</t>
+  </si>
+  <si>
+    <t>with command mongodb: db.stats()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - db (string): the name of the database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - collections (number): the number of collections in that database. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - objects (number): the number of objects in the database across all collections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - avgObjSize (bytes): The average size of each document in bytes. This is the dataSize divided by the number of documents.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - dataSize (bytes): The total size in bytes of the data held in this database including the padding factor. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - storageSize (bytes): The total amount of space in bytes allocated to collections in this database for document storage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - numExtents (number): the number of extents in the database across all collections.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - indexes (number): the total number of indexes across all collections in the database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - indexSize (bytes): The total size in bytes of all indexes created on this database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - fileSize (bytes): The total size in bytes of the data files that hold the database. This value includes preallocated space and the padding factor. The value of fileSize only reflects the size of the data files for the database and not the namespace file.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - nsSizeMB (MB): The total size of the namespace files for this database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - dataFileVersion: information about the on-disk format of the data files for the database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + minor (number): The minor version number for the on-disk format of the data files for the database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + major (number): The major version number for the on-disk format of the data files for the database.</t>
+  </si>
+  <si>
+    <t>MongoDB.Statistics.DatabaseInfo</t>
+  </si>
+  <si>
+    <t>4. Monitoring statistics for a given collection</t>
+  </si>
+  <si>
+    <t>Monitoring statistics for a given collection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +587,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -446,7 +626,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -742,44 +922,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:C6"/>
+  <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="16.5">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
     </row>
     <row r="4" spans="2:3">
-      <c r="B4" s="2"/>
       <c r="C4" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-    </row>
     <row r="6" spans="2:3">
-      <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
         <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="C8" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" s="6" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C4" location="ServerStatus!B2" display="1. Monitoring information of server"/>
     <hyperlink ref="C6" location="HostInfo!B2" display="2. Monitoring host information"/>
+    <hyperlink ref="C8" location="dbStats!B2" display="Monitoring statistics for a given database"/>
+    <hyperlink ref="C10" location="'collectionStats '!B2" display="4. Monitoring statistics for a given collection"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -790,7 +974,7 @@
   <dimension ref="B2:H136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -806,7 +990,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="15">
+    <row r="3" spans="2:8">
       <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1418,23 +1602,286 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="16.5">
+      <c r="B2" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="C3" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="C6" s="5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="D7" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="D8" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="D9" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="D10" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="D11" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="D12" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="D13" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="C15" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="D16" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="D17" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="D18" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4">
+      <c r="C20" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="D21" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="D22" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="D23" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="3:4">
+      <c r="D24" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4">
+      <c r="D25" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="3:4">
+      <c r="D26" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4">
+      <c r="D27" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4">
+      <c r="D28" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="16.5">
+      <c r="B2" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="C3" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="C4" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="C6" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="D7" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="D8" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="D9" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="D10" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="D11" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="D12" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="D13" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="D14" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="D15" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="D16" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5">
+      <c r="D17" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5">
+      <c r="D18" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5">
+      <c r="E19" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5">
+      <c r="E20" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" location="dbcmd.dbStats"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="16.5">
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>